<commit_message>
entity and property prep work for ontology implementation
</commit_message>
<xml_diff>
--- a/vocabulary/iSample-SampleMetadataProperties.xlsx
+++ b/vocabulary/iSample-SampleMetadataProperties.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D476615F-6086-4DF4-8A6C-DD570B8A2C9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50D0F46-A8D3-4167-9E5E-AF59A7ABBF37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12375" yWindow="1440" windowWidth="14280" windowHeight="14295" firstSheet="1" activeTab="3" xr2:uid="{E43F2E3F-723B-4F10-9D5E-20804E2FA629}"/>
-    <workbookView xWindow="9255" yWindow="750" windowWidth="20625" windowHeight="12540" activeTab="1" xr2:uid="{3680DB5C-442F-4389-AB6B-E77EE702B503}"/>
+    <workbookView xWindow="11265" yWindow="750" windowWidth="16365" windowHeight="13605" firstSheet="1" activeTab="3" xr2:uid="{E43F2E3F-723B-4F10-9D5E-20804E2FA629}"/>
   </bookViews>
   <sheets>
     <sheet name="ESS-DIVE mapping" sheetId="1" r:id="rId1"/>
@@ -1572,7 +1571,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1635,12 +1634,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1729,9 +1722,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1790,7 +1780,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1801,6 +1791,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2139,9 +2132,6 @@
     <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
-    <sheetView topLeftCell="A20" workbookViewId="1">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2174,7 +2164,7 @@
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2190,7 +2180,7 @@
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -2215,7 +2205,7 @@
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2232,7 +2222,7 @@
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2271,7 +2261,7 @@
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -2285,7 +2275,7 @@
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2296,7 +2286,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -2369,7 +2359,7 @@
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2422,7 +2412,7 @@
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2456,7 +2446,7 @@
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>383</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -2470,7 +2460,7 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>390</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -2495,7 +2485,7 @@
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -2531,7 +2521,7 @@
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2553,7 +2543,7 @@
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -2567,7 +2557,7 @@
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -2581,7 +2571,7 @@
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="2" t="s">
@@ -2611,11 +2601,11 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -2690,11 +2680,11 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
       <c r="F49" s="2" t="s">
         <v>86</v>
       </c>
@@ -2725,7 +2715,7 @@
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2788,10 +2778,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="6" t="s">
         <v>137</v>
       </c>
       <c r="F65" s="2" t="s">
@@ -2928,9 +2918,6 @@
     <sheetView topLeftCell="D104" workbookViewId="0">
       <selection activeCell="E126" sqref="E126"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="1">
-      <selection activeCell="F80" sqref="F80"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2943,24 +2930,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>155</v>
       </c>
       <c r="C2" s="1"/>
@@ -2970,7 +2957,7 @@
     </row>
     <row r="3" spans="2:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>176</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2982,7 +2969,7 @@
     </row>
     <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2997,7 +2984,7 @@
     </row>
     <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3027,7 +3014,7 @@
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -3042,7 +3029,7 @@
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3057,7 +3044,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>306</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -3071,13 +3058,13 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>406</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -3116,7 +3103,7 @@
     </row>
     <row r="13" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -3131,7 +3118,7 @@
     </row>
     <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>307</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3146,7 +3133,7 @@
     </row>
     <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>309</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -3161,7 +3148,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>308</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -3175,12 +3162,12 @@
       </c>
     </row>
     <row r="17" spans="2:6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="18" spans="2:6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>410</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3194,7 +3181,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>485</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -3209,7 +3196,7 @@
     </row>
     <row r="20" spans="2:6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>219</v>
       </c>
       <c r="C21" s="1"/>
@@ -3263,7 +3250,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -3307,7 +3294,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="28" t="s">
         <v>314</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -3377,7 +3364,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="25" t="s">
         <v>68</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -3396,7 +3383,7 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="30" t="s">
         <v>332</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -3418,7 +3405,7 @@
       </c>
     </row>
     <row r="40" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="28" t="s">
         <v>334</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -3471,7 +3458,7 @@
       </c>
     </row>
     <row r="45" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>149</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -3490,7 +3477,7 @@
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="28" t="s">
         <v>321</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -3526,7 +3513,7 @@
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="28" t="s">
         <v>151</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -3540,7 +3527,7 @@
       </c>
     </row>
     <row r="52" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3561,7 +3548,7 @@
     </row>
     <row r="54" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B54"/>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="28" t="s">
         <v>324</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -3575,7 +3562,7 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="28" t="s">
         <v>325</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -3589,7 +3576,7 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="28" t="s">
         <v>326</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -3631,7 +3618,7 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3647,7 +3634,7 @@
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="28" t="s">
         <v>328</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -3697,7 +3684,7 @@
       </c>
     </row>
     <row r="67" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="25" t="s">
         <v>143</v>
       </c>
       <c r="F67" s="2" t="s">
@@ -3716,7 +3703,7 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="28" t="s">
         <v>317</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -3777,7 +3764,7 @@
       </c>
     </row>
     <row r="75" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="25" t="s">
         <v>141</v>
       </c>
       <c r="F75" s="2" t="s">
@@ -3796,7 +3783,7 @@
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="28" t="s">
         <v>310</v>
       </c>
       <c r="D77" s="2" t="s">
@@ -3807,7 +3794,7 @@
       </c>
     </row>
     <row r="78" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="28" t="s">
         <v>311</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -3818,7 +3805,7 @@
       </c>
     </row>
     <row r="80" spans="2:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="26" t="s">
+      <c r="B80" s="25" t="s">
         <v>153</v>
       </c>
       <c r="E80" s="2" t="s">
@@ -3868,7 +3855,7 @@
       </c>
     </row>
     <row r="84" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B84" s="12"/>
+      <c r="B84" s="11"/>
       <c r="C84" s="2" t="s">
         <v>78</v>
       </c>
@@ -3883,8 +3870,8 @@
       </c>
     </row>
     <row r="85" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="12"/>
-      <c r="C85" s="29" t="s">
+      <c r="B85" s="11"/>
+      <c r="C85" s="28" t="s">
         <v>302</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3898,10 +3885,10 @@
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="12"/>
+      <c r="B86" s="11"/>
     </row>
     <row r="87" spans="2:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="12" t="s">
         <v>296</v>
       </c>
       <c r="F87" s="2" t="s">
@@ -3967,7 +3954,7 @@
       <c r="B92"/>
     </row>
     <row r="93" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="12" t="s">
         <v>189</v>
       </c>
       <c r="F93" s="2" t="s">
@@ -4059,7 +4046,7 @@
       </c>
     </row>
     <row r="101" spans="2:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="12" t="s">
         <v>197</v>
       </c>
       <c r="F101" s="2" t="s">
@@ -4140,7 +4127,7 @@
       <c r="B108"/>
     </row>
     <row r="109" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="8" t="s">
         <v>384</v>
       </c>
       <c r="F109" s="2" t="s">
@@ -4148,7 +4135,7 @@
       </c>
     </row>
     <row r="110" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C110" s="29" t="s">
+      <c r="C110" s="28" t="s">
         <v>255</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -4162,7 +4149,7 @@
       </c>
     </row>
     <row r="111" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C111" s="29" t="s">
+      <c r="C111" s="28" t="s">
         <v>342</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4176,7 +4163,7 @@
       </c>
     </row>
     <row r="113" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="26" t="s">
+      <c r="B113" s="25" t="s">
         <v>181</v>
       </c>
       <c r="F113" s="2" t="s">
@@ -4184,7 +4171,7 @@
       </c>
     </row>
     <row r="114" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="29" t="s">
+      <c r="C114" s="28" t="s">
         <v>185</v>
       </c>
       <c r="D114" s="2" t="s">
@@ -4209,7 +4196,7 @@
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="29" t="s">
+      <c r="C116" s="28" t="s">
         <v>187</v>
       </c>
       <c r="D116" s="2" t="s">
@@ -4253,7 +4240,7 @@
     <row r="121" spans="2:6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="2:6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="26" t="s">
+      <c r="B123" s="25" t="s">
         <v>371</v>
       </c>
       <c r="F123" s="2" t="s">
@@ -4274,7 +4261,7 @@
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125"/>
-      <c r="C125" s="29" t="s">
+      <c r="C125" s="28" t="s">
         <v>271</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4309,7 +4296,7 @@
       </c>
     </row>
     <row r="129" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="26" t="s">
+      <c r="B129" s="25" t="s">
         <v>368</v>
       </c>
       <c r="F129" s="2" t="s">
@@ -4328,7 +4315,7 @@
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C131" s="29" t="s">
+      <c r="C131" s="28" t="s">
         <v>267</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -4372,7 +4359,7 @@
       </c>
     </row>
     <row r="136" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="26" t="s">
+      <c r="B136" s="25" t="s">
         <v>383</v>
       </c>
       <c r="F136" s="2" t="s">
@@ -4381,7 +4368,7 @@
     </row>
     <row r="137" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B137"/>
-      <c r="C137" s="29" t="s">
+      <c r="C137" s="28" t="s">
         <v>226</v>
       </c>
       <c r="D137" s="2" t="s">
@@ -4392,7 +4379,7 @@
       </c>
     </row>
     <row r="138" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C138" s="29" t="s">
+      <c r="C138" s="28" t="s">
         <v>260</v>
       </c>
       <c r="D138" s="2" t="s">
@@ -4406,7 +4393,7 @@
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C139" s="29" t="s">
+      <c r="C139" s="28" t="s">
         <v>262</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -4420,7 +4407,7 @@
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C140" s="29" t="s">
+      <c r="C140" s="28" t="s">
         <v>263</v>
       </c>
       <c r="D140" s="2" t="s">
@@ -4434,12 +4421,12 @@
       <c r="B141"/>
     </row>
     <row r="142" spans="2:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="8" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="143" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C143" s="30" t="s">
+      <c r="C143" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D143" s="2" t="s">
@@ -4453,7 +4440,7 @@
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="29" t="s">
+      <c r="C144" s="28" t="s">
         <v>226</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -4467,7 +4454,7 @@
       </c>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C145" s="29" t="s">
+      <c r="C145" s="28" t="s">
         <v>49</v>
       </c>
       <c r="D145" s="2" t="s">
@@ -4481,7 +4468,7 @@
       </c>
     </row>
     <row r="147" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="9" t="s">
+      <c r="B147" s="8" t="s">
         <v>484</v>
       </c>
       <c r="F147" s="2" t="s">
@@ -4489,7 +4476,7 @@
       </c>
     </row>
     <row r="148" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C148" s="29" t="s">
+      <c r="C148" s="28" t="s">
         <v>255</v>
       </c>
       <c r="D148" s="2" t="s">
@@ -4500,7 +4487,7 @@
       </c>
     </row>
     <row r="149" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C149" s="29" t="s">
+      <c r="C149" s="28" t="s">
         <v>471</v>
       </c>
       <c r="D149" s="2" t="s">
@@ -4535,7 +4522,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4545,7 +4531,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>343</v>
       </c>
       <c r="B1" t="s">
@@ -4556,7 +4542,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>364</v>
       </c>
     </row>
@@ -4610,7 +4596,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>362</v>
       </c>
     </row>
@@ -4635,7 +4621,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>363</v>
       </c>
     </row>
@@ -4673,7 +4659,7 @@
       <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="16"/>
     </row>
     <row r="33" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -4703,7 +4689,7 @@
       <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -4721,7 +4707,7 @@
       <c r="A47" s="2"/>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
+      <c r="A50" s="18"/>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -4742,7 +4728,7 @@
       <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16"/>
+      <c r="A57" s="15"/>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -4766,7 +4752,7 @@
       <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16"/>
+      <c r="A65" s="15"/>
     </row>
     <row r="66" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
@@ -4781,7 +4767,7 @@
       <c r="A69" s="2"/>
     </row>
     <row r="72" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
+      <c r="A72" s="15"/>
     </row>
     <row r="73" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
@@ -4805,7 +4791,7 @@
       <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="16"/>
+      <c r="A80" s="15"/>
     </row>
     <row r="81" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
@@ -4826,7 +4812,7 @@
       <c r="A86" s="2"/>
     </row>
     <row r="87" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="20"/>
+      <c r="A87" s="19"/>
     </row>
     <row r="88" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
@@ -4844,13 +4830,13 @@
       <c r="A92" s="2"/>
     </row>
     <row r="93" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="18"/>
+      <c r="A93" s="17"/>
     </row>
     <row r="94" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
+      <c r="A94" s="11"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
+      <c r="A95" s="11"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
@@ -4859,7 +4845,7 @@
       <c r="A97" s="2"/>
     </row>
     <row r="101" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="20"/>
+      <c r="A101" s="19"/>
     </row>
     <row r="102" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
@@ -4883,11 +4869,11 @@
       <c r="A108" s="2"/>
     </row>
     <row r="109" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="16"/>
+      <c r="A109" s="15"/>
     </row>
     <row r="110" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="19"/>
+      <c r="A114" s="18"/>
     </row>
     <row r="115" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
@@ -4902,7 +4888,7 @@
       <c r="A118" s="2"/>
     </row>
     <row r="120" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="16"/>
+      <c r="A120" s="15"/>
     </row>
     <row r="121" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
@@ -4920,7 +4906,7 @@
       <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="16"/>
+      <c r="A126" s="15"/>
     </row>
     <row r="127" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
@@ -4929,7 +4915,7 @@
       <c r="A128" s="2"/>
     </row>
     <row r="132" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="19"/>
+      <c r="A132" s="18"/>
     </row>
     <row r="133" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
@@ -4942,7 +4928,7 @@
       <c r="A136" s="2"/>
     </row>
     <row r="137" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="16"/>
+      <c r="A137" s="15"/>
     </row>
     <row r="138" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
@@ -4969,9 +4955,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView topLeftCell="A52" workbookViewId="1">
-      <selection activeCell="D57" sqref="D57"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4983,16 +4966,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>467</v>
       </c>
     </row>
@@ -5133,7 +5116,7 @@
       <c r="B13" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>424</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -5713,9 +5696,6 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5724,10 +5704,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>349</v>
       </c>
     </row>
@@ -5852,7 +5832,7 @@
       </c>
     </row>
     <row r="21" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6269,9 +6249,6 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>